<commit_message>
retirando spacos do cota extra
</commit_message>
<xml_diff>
--- a/PLANILHA TESTE.xlsx
+++ b/PLANILHA TESTE.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guido\Desktop\GitHub Repositories\PrimeiroBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFA6F7A-0ECD-42FC-B11D-444640C388EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FCFBA7-FC3B-4B20-9A6D-FE5CA9672E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="0" windowWidth="12150" windowHeight="10905" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14955" yWindow="-975" windowWidth="12150" windowHeight="10905" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pedidos" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="a" localSheetId="0">Pedidos!$A$1:$S$53</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Pedidos!$A$1:$S$53</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -1151,27 +1151,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1180,6 +1159,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1520,9 +1520,9 @@
   </sheetPr>
   <dimension ref="A1:BN114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,7 +1816,9 @@
       <c r="K9" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="37"/>
+      <c r="L9" s="37">
+        <v>5</v>
+      </c>
       <c r="M9" s="38" t="s">
         <v>30</v>
       </c>
@@ -1859,7 +1861,9 @@
       <c r="K10" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="37"/>
+      <c r="L10" s="37">
+        <v>5</v>
+      </c>
       <c r="M10" s="38" t="s">
         <v>37</v>
       </c>
@@ -1900,7 +1904,9 @@
       <c r="K11" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="37"/>
+      <c r="L11" s="37">
+        <v>5</v>
+      </c>
       <c r="M11" s="38" t="s">
         <v>46</v>
       </c>
@@ -6257,117 +6263,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67"/>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68" t="s">
+      <c r="A1" s="60"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
     </row>
     <row r="4" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64" t="s">
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="64"/>
+      <c r="F4" s="63"/>
       <c r="G4" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64" t="s">
+      <c r="I4" s="63"/>
+      <c r="J4" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64" t="s">
+      <c r="K4" s="63"/>
+      <c r="L4" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="64"/>
+      <c r="M4" s="63"/>
     </row>
     <row r="5" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60">
+      <c r="A5" s="64">
         <v>1</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="66" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="66"/>
+      <c r="F5" s="65"/>
       <c r="G5" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="60" t="s">
+      <c r="H5" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60" t="s">
+      <c r="I5" s="64"/>
+      <c r="J5" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60" t="s">
+      <c r="K5" s="64"/>
+      <c r="L5" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="M5" s="60"/>
+      <c r="M5" s="64"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
       <c r="G6" s="44"/>
       <c r="H6" s="45"/>
       <c r="I6" s="45"/>
@@ -6377,91 +6383,109 @@
       <c r="M6" s="45"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64" t="s">
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="65" t="s">
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60">
+      <c r="A8" s="64">
         <v>0</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="61">
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="68">
         <v>43009</v>
       </c>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62" t="s">
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60">
+      <c r="A9" s="64">
         <v>1</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="61">
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="68">
         <v>45238</v>
       </c>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62" t="s">
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60">
+      <c r="A10" s="64">
         <v>2</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61">
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="68">
         <v>45405</v>
       </c>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62" t="s">
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:M9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:M10"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
     <mergeCell ref="A1:D3"/>
     <mergeCell ref="E1:I3"/>
     <mergeCell ref="J1:M3"/>
@@ -6470,24 +6494,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:M9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:M10"/>
   </mergeCells>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>